<commit_message>
chore: Refactor image handling, sword movement, and rectangle functionality
Refactor the code for image handling, sword movement, and drag and drop functionality for rectangles. This commit improves the organization and structure of the code related to these features.

The changes are made in the `test3.py` file.
</commit_message>
<xml_diff>
--- a/excel/game_scores.xlsx
+++ b/excel/game_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,76 @@
         <v>116</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-211810.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-212021.png</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-212129.png</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-214041.png</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-215840.png</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-215947.png</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-220054.png</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Improve image handling, sword movement, and rectangle functionality
</commit_message>
<xml_diff>
--- a/excel/game_scores.xlsx
+++ b/excel/game_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,6 +525,166 @@
         <v>53</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240713-234946.png</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-000050.png</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-000341.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-001913.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-002019.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-002138.png</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-002309.png</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-002851.png</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-005014.png</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-005124.png</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-005320.png</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-005449.png</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-005816.png</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-010859.png</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-011315.png</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>./img/player_image_20240714-011814.png</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>